<commit_message>
updates for 1 apr done adding data from world o meter
</commit_message>
<xml_diff>
--- a/Case Estimate by German Rate.xlsx
+++ b/Case Estimate by German Rate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{FE0DE54D-1230-4A0D-9807-4F862C3D0BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C54C289-76FA-4A04-AC3F-DE39F9953F66}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13BB10E1-65F4-4F98-A4B5-4406EB562241}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="21270" yWindow="-12330" windowWidth="10395" windowHeight="16290" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -52,15 +53,22 @@
   <si>
     <t>Germany</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Confirmed Cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -100,12 +108,15 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -424,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C06F9B-DBEB-497F-9724-20C3DD10AC15}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -483,4 +494,1800 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
+  <dimension ref="A1:E94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72:E94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43830</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="e">
+        <f>C2/B2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E2" t="e">
+        <f>1/D2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>43831</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="e">
+        <f t="shared" ref="D3:D66" si="0">C3/B3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E3" t="e">
+        <f t="shared" ref="E3:E66" si="1">1/D3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>43832</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>43833</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>43834</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>43835</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>43836</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>43837</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>43838</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>43839</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>43840</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>43841</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>43842</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>43843</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>43844</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>43845</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>43846</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>43847</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>43848</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>43849</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <v>43850</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>43851</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>43852</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <v>43853</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
+        <v>43854</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <v>43855</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <v>43856</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5">
+        <v>43857</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
+        <v>43858</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>43859</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
+        <v>43860</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
+        <v>43861</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
+        <v>43862</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <v>43863</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
+        <v>43864</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
+        <v>43865</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
+        <v>43866</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="5">
+        <v>43867</v>
+      </c>
+      <c r="B39">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="5">
+        <v>43868</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="5">
+        <v>43869</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E41" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="5">
+        <v>43870</v>
+      </c>
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="5">
+        <v>43871</v>
+      </c>
+      <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="5">
+        <v>43872</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
+        <v>43873</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E45" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="5">
+        <v>43874</v>
+      </c>
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E46" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="5">
+        <v>43875</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="5">
+        <v>43876</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E48" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="5">
+        <v>43877</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="5">
+        <v>43878</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E50" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="5">
+        <v>43879</v>
+      </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E51" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
+        <v>43880</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E52" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
+        <v>43881</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E53" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
+        <v>43882</v>
+      </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E54" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
+        <v>43883</v>
+      </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E55" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="5">
+        <v>43884</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E56" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="5">
+        <v>43885</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E57" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="5">
+        <v>43886</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E58" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B59">
+        <v>17</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E59" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="5">
+        <v>43888</v>
+      </c>
+      <c r="B60">
+        <v>21</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E60" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="5">
+        <v>43889</v>
+      </c>
+      <c r="B61">
+        <v>47</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E61" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="5">
+        <v>43890</v>
+      </c>
+      <c r="B62">
+        <v>57</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E62" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="5">
+        <v>43891</v>
+      </c>
+      <c r="B63">
+        <v>111</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E63" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="5">
+        <v>43892</v>
+      </c>
+      <c r="B64">
+        <v>129</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E64" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="5">
+        <v>43893</v>
+      </c>
+      <c r="B65">
+        <v>157</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E65" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="5">
+        <v>43894</v>
+      </c>
+      <c r="B66">
+        <v>196</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E66" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="5">
+        <v>43895</v>
+      </c>
+      <c r="B67">
+        <v>262</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" ref="D67:D92" si="2">C67/B67</f>
+        <v>0</v>
+      </c>
+      <c r="E67" t="e">
+        <f t="shared" ref="E67:E94" si="3">1/D67</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="5">
+        <v>43896</v>
+      </c>
+      <c r="B68">
+        <v>400</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E68" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
+        <v>43897</v>
+      </c>
+      <c r="B69">
+        <v>684</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E69" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="5">
+        <v>43898</v>
+      </c>
+      <c r="B70">
+        <v>847</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E70" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="5">
+        <v>43899</v>
+      </c>
+      <c r="B71">
+        <v>902</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E71" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="5">
+        <v>43900</v>
+      </c>
+      <c r="B72">
+        <v>1139</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7559262510974539E-3</v>
+      </c>
+      <c r="E72" s="7">
+        <f t="shared" si="3"/>
+        <v>569.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="5">
+        <v>43901</v>
+      </c>
+      <c r="B73">
+        <v>1296</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5432098765432098E-3</v>
+      </c>
+      <c r="E73" s="7">
+        <f t="shared" si="3"/>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="5">
+        <v>43902</v>
+      </c>
+      <c r="B74">
+        <v>1567</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9144862795149968E-3</v>
+      </c>
+      <c r="E74" s="7">
+        <f t="shared" si="3"/>
+        <v>522.33333333333337</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="5">
+        <v>43903</v>
+      </c>
+      <c r="B75">
+        <v>2369</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1105951878429719E-3</v>
+      </c>
+      <c r="E75" s="7">
+        <f t="shared" si="3"/>
+        <v>473.79999999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="5">
+        <v>43904</v>
+      </c>
+      <c r="B76">
+        <v>3062</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6329196603527107E-3</v>
+      </c>
+      <c r="E76" s="7">
+        <f t="shared" si="3"/>
+        <v>612.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="5">
+        <v>43905</v>
+      </c>
+      <c r="B77">
+        <v>3795</v>
+      </c>
+      <c r="C77">
+        <v>8</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1080368906455861E-3</v>
+      </c>
+      <c r="E77" s="7">
+        <f t="shared" si="3"/>
+        <v>474.37500000000006</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="5">
+        <v>43906</v>
+      </c>
+      <c r="B78">
+        <v>4838</v>
+      </c>
+      <c r="C78">
+        <v>12</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="2"/>
+        <v>2.4803637866887144E-3</v>
+      </c>
+      <c r="E78" s="7">
+        <f t="shared" si="3"/>
+        <v>403.16666666666669</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="5">
+        <v>43907</v>
+      </c>
+      <c r="B79">
+        <v>6012</v>
+      </c>
+      <c r="C79">
+        <v>13</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="2"/>
+        <v>2.162341982701264E-3</v>
+      </c>
+      <c r="E79" s="7">
+        <f t="shared" si="3"/>
+        <v>462.46153846153851</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="5">
+        <v>43908</v>
+      </c>
+      <c r="B80">
+        <v>7156</v>
+      </c>
+      <c r="C80">
+        <v>13</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8166573504751259E-3</v>
+      </c>
+      <c r="E80" s="7">
+        <f t="shared" si="3"/>
+        <v>550.46153846153845</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="5">
+        <v>43909</v>
+      </c>
+      <c r="B81">
+        <v>8198</v>
+      </c>
+      <c r="C81">
+        <v>13</v>
+      </c>
+      <c r="D81" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5857526225908757E-3</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="3"/>
+        <v>630.61538461538464</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="5">
+        <v>43910</v>
+      </c>
+      <c r="B82">
+        <v>14138</v>
+      </c>
+      <c r="C82">
+        <v>43</v>
+      </c>
+      <c r="D82" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0414485782996182E-3</v>
+      </c>
+      <c r="E82" s="7">
+        <f t="shared" si="3"/>
+        <v>328.7906976744186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="5">
+        <v>43911</v>
+      </c>
+      <c r="B83">
+        <v>18187</v>
+      </c>
+      <c r="C83">
+        <v>45</v>
+      </c>
+      <c r="D83" s="2">
+        <f t="shared" si="2"/>
+        <v>2.474294825974597E-3</v>
+      </c>
+      <c r="E83" s="7">
+        <f t="shared" si="3"/>
+        <v>404.15555555555557</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="5">
+        <v>43912</v>
+      </c>
+      <c r="B84">
+        <v>21463</v>
+      </c>
+      <c r="C84">
+        <v>67</v>
+      </c>
+      <c r="D84" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1216512137166286E-3</v>
+      </c>
+      <c r="E84" s="7">
+        <f t="shared" si="3"/>
+        <v>320.34328358208955</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="5">
+        <v>43913</v>
+      </c>
+      <c r="B85">
+        <v>24774</v>
+      </c>
+      <c r="C85">
+        <v>94</v>
+      </c>
+      <c r="D85" s="2">
+        <f t="shared" si="2"/>
+        <v>3.7943004763058043E-3</v>
+      </c>
+      <c r="E85" s="7">
+        <f t="shared" si="3"/>
+        <v>263.55319148936172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="5">
+        <v>43914</v>
+      </c>
+      <c r="B86">
+        <v>29212</v>
+      </c>
+      <c r="C86">
+        <v>126</v>
+      </c>
+      <c r="D86" s="2">
+        <f t="shared" si="2"/>
+        <v>4.3132959057921401E-3</v>
+      </c>
+      <c r="E86" s="7">
+        <f t="shared" si="3"/>
+        <v>231.84126984126985</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="5">
+        <v>43915</v>
+      </c>
+      <c r="B87">
+        <v>31554</v>
+      </c>
+      <c r="C87">
+        <v>149</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7220637637066616E-3</v>
+      </c>
+      <c r="E87" s="7">
+        <f t="shared" si="3"/>
+        <v>211.7718120805369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="5">
+        <v>43916</v>
+      </c>
+      <c r="B88">
+        <v>36508</v>
+      </c>
+      <c r="C88">
+        <v>198</v>
+      </c>
+      <c r="D88" s="2">
+        <f t="shared" si="2"/>
+        <v>5.4234688287498629E-3</v>
+      </c>
+      <c r="E88" s="7">
+        <f t="shared" si="3"/>
+        <v>184.38383838383839</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="5">
+        <v>43917</v>
+      </c>
+      <c r="B89">
+        <v>42288</v>
+      </c>
+      <c r="C89">
+        <v>253</v>
+      </c>
+      <c r="D89" s="2">
+        <f t="shared" si="2"/>
+        <v>5.9827847143397658E-3</v>
+      </c>
+      <c r="E89" s="7">
+        <f t="shared" si="3"/>
+        <v>167.14624505928853</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="5">
+        <v>43918</v>
+      </c>
+      <c r="B90">
+        <v>48582</v>
+      </c>
+      <c r="C90">
+        <v>325</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" si="2"/>
+        <v>6.6897204726030215E-3</v>
+      </c>
+      <c r="E90" s="7">
+        <f t="shared" si="3"/>
+        <v>149.48307692307694</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="5">
+        <v>43919</v>
+      </c>
+      <c r="B91">
+        <v>52547</v>
+      </c>
+      <c r="C91">
+        <v>389</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4028964546025465E-3</v>
+      </c>
+      <c r="E91" s="7">
+        <f t="shared" si="3"/>
+        <v>135.0822622107969</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="5">
+        <v>43920</v>
+      </c>
+      <c r="B92">
+        <v>57298</v>
+      </c>
+      <c r="C92">
+        <v>455</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9409403469580097E-3</v>
+      </c>
+      <c r="E92" s="7">
+        <f t="shared" si="3"/>
+        <v>125.92967032967032</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="5">
+        <v>43921</v>
+      </c>
+      <c r="B93">
+        <v>67051</v>
+      </c>
+      <c r="C93">
+        <v>650</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" ref="D93:D94" si="4">C93/B93</f>
+        <v>9.694113436041223E-3</v>
+      </c>
+      <c r="E93" s="7">
+        <f t="shared" si="3"/>
+        <v>103.15538461538461</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="5">
+        <v>43922</v>
+      </c>
+      <c r="B94">
+        <v>72383</v>
+      </c>
+      <c r="C94">
+        <v>788</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0886534130942349E-2</v>
+      </c>
+      <c r="E94" s="7">
+        <f t="shared" si="3"/>
+        <v>91.856598984771566</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for 2 Ap
</commit_message>
<xml_diff>
--- a/Case Estimate by German Rate.xlsx
+++ b/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13BB10E1-65F4-4F98-A4B5-4406EB562241}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38046D00-CCC7-486A-B6C1-ADF9C404ABE2}"/>
   <bookViews>
-    <workbookView xWindow="21270" yWindow="-12330" windowWidth="10395" windowHeight="16290" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="18570" yWindow="-20655" windowWidth="18915" windowHeight="16290" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72:E94"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E94" si="3">1/D67</f>
+        <f t="shared" ref="E67:E95" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D94" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D95" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2285,6 +2285,25 @@
       <c r="E94" s="7">
         <f t="shared" si="3"/>
         <v>91.856598984771566</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="5">
+        <v>43923</v>
+      </c>
+      <c r="B95">
+        <v>78115</v>
+      </c>
+      <c r="C95">
+        <v>944</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2084746847596492E-2</v>
+      </c>
+      <c r="E95" s="7">
+        <f t="shared" si="3"/>
+        <v>82.748940677966104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 3 April
</commit_message>
<xml_diff>
--- a/Case Estimate by German Rate.xlsx
+++ b/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38046D00-CCC7-486A-B6C1-ADF9C404ABE2}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{90735363-E9B3-4842-AE9E-B6836EAD0E57}"/>
   <bookViews>
-    <workbookView xWindow="18570" yWindow="-20655" windowWidth="18915" windowHeight="16290" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="19515" yWindow="-19065" windowWidth="27615" windowHeight="16290" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="J89" sqref="J89"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E95" si="3">1/D67</f>
+        <f t="shared" ref="E67:E96" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D95" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D96" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2304,6 +2304,25 @@
       <c r="E95" s="7">
         <f t="shared" si="3"/>
         <v>82.748940677966104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="5">
+        <v>43924</v>
+      </c>
+      <c r="B96">
+        <v>85063</v>
+      </c>
+      <c r="C96">
+        <v>1111</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3060907797749903E-2</v>
+      </c>
+      <c r="E96" s="7">
+        <f t="shared" si="3"/>
+        <v>76.56435643564356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>